<commit_message>
Commit done on 5th May 2023
</commit_message>
<xml_diff>
--- a/testdata/LoginData.xlsx
+++ b/testdata/LoginData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nithya\PycharmProjects\nopecommerceApp\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nithya\PycharmProjects\Automationproject\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C85B95AC-F5C0-47A6-919E-DF5F592C5F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18950DDC-57DA-4A15-B54B-A4DEB807699B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="1035" windowWidth="13035" windowHeight="11385" xr2:uid="{99041768-BCFD-43D6-944C-AF7D37D4EDA9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{99041768-BCFD-43D6-944C-AF7D37D4EDA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>username</t>
   </si>
@@ -47,22 +47,10 @@
     <t>exp</t>
   </si>
   <si>
-    <t>admin@yourstore.com</t>
+    <t>notification.testing@novasignal.com</t>
   </si>
   <si>
-    <t>adm@yourstore.com</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>adm</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
+    <t>novasignal</t>
   </si>
 </sst>
 </file>
@@ -437,13 +425,13 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="B3" sqref="A3:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -463,53 +451,23 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
+      <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
+      <c r="A5" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{4DB0DC7C-CB07-46D5-80C1-4DA499944880}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{0D3FA373-787F-4895-9E2C-B3B123FFEE0B}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{BF79905B-971A-4D8D-B942-4E32AA215324}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{CFF1C07D-7B93-4F58-A8D1-197A077AA9DD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>